<commit_message>
euro tie break challenge
</commit_message>
<xml_diff>
--- a/data/tb_euro_fifa.xlsx
+++ b/data/tb_euro_fifa.xlsx
@@ -1816,13 +1816,13 @@
         <v>1</v>
       </c>
       <c r="F46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" t="n">
         <v>0</v>
       </c>
       <c r="H46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -1879,10 +1879,10 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -4896,11 +4896,11 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E149" t="n">
         <v>1</v>
@@ -4912,7 +4912,7 @@
         <v>0</v>
       </c>
       <c r="H149" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150">
@@ -4926,20 +4926,20 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E150" t="n">
         <v>2</v>
       </c>
       <c r="F150" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G150" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H150" t="n">
         <v>4</v>
@@ -4956,23 +4956,23 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>France</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E151" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F151" t="n">
         <v>2</v>
       </c>
       <c r="G151" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H151" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="152">
@@ -4993,16 +4993,16 @@
         <v>0</v>
       </c>
       <c r="E152" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F152" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G152" t="n">
         <v>2</v>
       </c>
       <c r="H152" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153">
@@ -5293,7 +5293,7 @@
         <v>0</v>
       </c>
       <c r="E162" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F162" t="n">
         <v>1</v>
@@ -5302,7 +5302,7 @@
         <v>0</v>
       </c>
       <c r="H162" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163">
@@ -5326,13 +5326,13 @@
         <v>1</v>
       </c>
       <c r="F163" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G163" t="n">
         <v>0</v>
       </c>
       <c r="H163" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164">
@@ -5359,10 +5359,10 @@
         <v>0</v>
       </c>
       <c r="G164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H164" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165">

</xml_diff>